<commit_message>
fetching max positions per complex
</commit_message>
<xml_diff>
--- a/misc/TUCres.xlsx
+++ b/misc/TUCres.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26924"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26827"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\aris\Projects\TUChome\misc\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\djari\Documents\Projects\TUChome\misc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B413AF89-87D2-405C-AD71-08ADC41462A3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{84F2B1A8-86DF-4AE4-B0B4-39F776B2784D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Φύλλο1" sheetId="3" r:id="rId1"/>
@@ -2348,42 +2348,42 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4F51C053-75FC-4752-8299-A2C139F86652}">
   <dimension ref="A1:Z181"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="I1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A51" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="V67" sqref="V67"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="6.5703125" style="11" customWidth="1"/>
+    <col min="1" max="1" width="6.5546875" style="11" customWidth="1"/>
     <col min="2" max="2" width="14" style="11" customWidth="1"/>
-    <col min="3" max="3" width="9.140625" style="11" customWidth="1"/>
-    <col min="4" max="4" width="10.7109375" style="11" customWidth="1"/>
-    <col min="5" max="5" width="8.42578125" style="11" customWidth="1"/>
-    <col min="6" max="6" width="14.85546875" style="11" bestFit="1" customWidth="1"/>
-    <col min="7" max="8" width="17.5703125" style="11" customWidth="1"/>
-    <col min="9" max="9" width="15.85546875" style="11" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="13.42578125" style="11" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="14.42578125" style="11" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="10.85546875" style="11" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="14.85546875" style="11" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="16.85546875" style="11" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="17.85546875" style="11" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="17.85546875" style="11" customWidth="1"/>
-    <col min="17" max="17" width="13.28515625" style="12" customWidth="1"/>
-    <col min="18" max="18" width="13.85546875" style="11" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="11.5703125" style="11" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="19.42578125" style="11" customWidth="1"/>
-    <col min="21" max="21" width="8.28515625" style="11" customWidth="1"/>
-    <col min="22" max="22" width="12.28515625" style="11" customWidth="1"/>
+    <col min="3" max="3" width="9.109375" style="11" customWidth="1"/>
+    <col min="4" max="4" width="10.6640625" style="11" customWidth="1"/>
+    <col min="5" max="5" width="8.44140625" style="11" customWidth="1"/>
+    <col min="6" max="6" width="14.88671875" style="11" bestFit="1" customWidth="1"/>
+    <col min="7" max="8" width="17.5546875" style="11" customWidth="1"/>
+    <col min="9" max="9" width="15.88671875" style="11" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="13.44140625" style="11" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="14.44140625" style="11" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="10.88671875" style="11" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="14.88671875" style="11" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="16.88671875" style="11" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="17.88671875" style="11" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="17.88671875" style="11" customWidth="1"/>
+    <col min="17" max="17" width="13.33203125" style="12" customWidth="1"/>
+    <col min="18" max="18" width="13.88671875" style="11" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="11.5546875" style="11" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="19.44140625" style="11" customWidth="1"/>
+    <col min="21" max="21" width="8.33203125" style="11" customWidth="1"/>
+    <col min="22" max="22" width="12.33203125" style="11" customWidth="1"/>
     <col min="23" max="23" width="21" style="11" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="15.140625" style="11" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="20.28515625" style="11" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="15.109375" style="11" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="20.33203125" style="11" bestFit="1" customWidth="1"/>
     <col min="26" max="26" width="19" style="11" customWidth="1"/>
-    <col min="27" max="16384" width="9.140625" style="11"/>
+    <col min="27" max="16384" width="9.109375" style="11"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:26" ht="45" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:26" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A1" s="19" t="s">
         <v>0</v>
       </c>
@@ -2463,7 +2463,7 @@
         <v>523</v>
       </c>
     </row>
-    <row r="2" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A2" s="11">
         <v>1</v>
       </c>
@@ -2477,7 +2477,7 @@
         <v>1</v>
       </c>
       <c r="E2" s="11" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="F2" s="11">
         <v>2821037223</v>
@@ -2516,7 +2516,7 @@
         <v>527</v>
       </c>
     </row>
-    <row r="3" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A3" s="11">
         <v>2</v>
       </c>
@@ -2569,7 +2569,7 @@
         <v>527</v>
       </c>
     </row>
-    <row r="4" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A4" s="11">
         <v>3</v>
       </c>
@@ -2622,7 +2622,7 @@
         <v>527</v>
       </c>
     </row>
-    <row r="5" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A5" s="11">
         <v>4</v>
       </c>
@@ -2675,7 +2675,7 @@
         <v>527</v>
       </c>
     </row>
-    <row r="6" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A6" s="11">
         <v>5</v>
       </c>
@@ -2749,7 +2749,7 @@
         <v>526</v>
       </c>
     </row>
-    <row r="7" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A7" s="11">
         <v>6</v>
       </c>
@@ -2802,7 +2802,7 @@
         <v>527</v>
       </c>
     </row>
-    <row r="8" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A8" s="11">
         <v>7</v>
       </c>
@@ -2855,7 +2855,7 @@
         <v>527</v>
       </c>
     </row>
-    <row r="9" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A9" s="11">
         <v>8</v>
       </c>
@@ -2908,7 +2908,7 @@
         <v>527</v>
       </c>
     </row>
-    <row r="10" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A10" s="11">
         <v>9</v>
       </c>
@@ -2961,7 +2961,7 @@
         <v>527</v>
       </c>
     </row>
-    <row r="11" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A11" s="11">
         <v>10</v>
       </c>
@@ -3014,7 +3014,7 @@
         <v>527</v>
       </c>
     </row>
-    <row r="12" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A12" s="11">
         <v>11</v>
       </c>
@@ -3067,7 +3067,7 @@
         <v>527</v>
       </c>
     </row>
-    <row r="13" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A13" s="11">
         <v>12</v>
       </c>
@@ -3120,7 +3120,7 @@
         <v>527</v>
       </c>
     </row>
-    <row r="14" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A14" s="11">
         <v>13</v>
       </c>
@@ -3173,7 +3173,7 @@
         <v>527</v>
       </c>
     </row>
-    <row r="15" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A15" s="11">
         <v>14</v>
       </c>
@@ -3226,7 +3226,7 @@
         <v>527</v>
       </c>
     </row>
-    <row r="16" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A16" s="11">
         <v>15</v>
       </c>
@@ -3279,7 +3279,7 @@
         <v>527</v>
       </c>
     </row>
-    <row r="17" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A17" s="11">
         <v>16</v>
       </c>
@@ -3332,7 +3332,7 @@
         <v>527</v>
       </c>
     </row>
-    <row r="18" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A18" s="11">
         <v>17</v>
       </c>
@@ -3385,7 +3385,7 @@
         <v>527</v>
       </c>
     </row>
-    <row r="19" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A19" s="11">
         <v>18</v>
       </c>
@@ -3438,7 +3438,7 @@
         <v>527</v>
       </c>
     </row>
-    <row r="20" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A20" s="11">
         <v>19</v>
       </c>
@@ -3491,7 +3491,7 @@
         <v>527</v>
       </c>
     </row>
-    <row r="21" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A21" s="11">
         <v>20</v>
       </c>
@@ -3544,7 +3544,7 @@
         <v>527</v>
       </c>
     </row>
-    <row r="22" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A22" s="11">
         <v>21</v>
       </c>
@@ -3597,7 +3597,7 @@
         <v>527</v>
       </c>
     </row>
-    <row r="23" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A23" s="11">
         <v>22</v>
       </c>
@@ -3650,7 +3650,7 @@
         <v>527</v>
       </c>
     </row>
-    <row r="24" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A24" s="11">
         <v>23</v>
       </c>
@@ -3703,7 +3703,7 @@
         <v>527</v>
       </c>
     </row>
-    <row r="25" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A25" s="11">
         <v>24</v>
       </c>
@@ -3756,7 +3756,7 @@
         <v>527</v>
       </c>
     </row>
-    <row r="26" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A26" s="11">
         <v>25</v>
       </c>
@@ -3809,7 +3809,7 @@
         <v>527</v>
       </c>
     </row>
-    <row r="27" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A27" s="11">
         <v>26</v>
       </c>
@@ -3862,7 +3862,7 @@
         <v>527</v>
       </c>
     </row>
-    <row r="28" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A28" s="11">
         <v>27</v>
       </c>
@@ -3915,7 +3915,7 @@
         <v>527</v>
       </c>
     </row>
-    <row r="29" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A29" s="11">
         <v>28</v>
       </c>
@@ -3968,7 +3968,7 @@
         <v>527</v>
       </c>
     </row>
-    <row r="30" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A30" s="11">
         <v>29</v>
       </c>
@@ -4021,7 +4021,7 @@
         <v>527</v>
       </c>
     </row>
-    <row r="31" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A31" s="11">
         <v>30</v>
       </c>
@@ -4074,7 +4074,7 @@
         <v>527</v>
       </c>
     </row>
-    <row r="32" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A32" s="11">
         <v>31</v>
       </c>
@@ -4127,7 +4127,7 @@
         <v>527</v>
       </c>
     </row>
-    <row r="33" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A33" s="11">
         <v>32</v>
       </c>
@@ -4180,7 +4180,7 @@
         <v>527</v>
       </c>
     </row>
-    <row r="34" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A34" s="11">
         <v>33</v>
       </c>
@@ -4233,7 +4233,7 @@
         <v>527</v>
       </c>
     </row>
-    <row r="35" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A35" s="11">
         <v>34</v>
       </c>
@@ -4286,7 +4286,7 @@
         <v>527</v>
       </c>
     </row>
-    <row r="36" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A36" s="11">
         <v>35</v>
       </c>
@@ -4339,7 +4339,7 @@
         <v>527</v>
       </c>
     </row>
-    <row r="37" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A37" s="11">
         <v>36</v>
       </c>
@@ -4392,7 +4392,7 @@
         <v>527</v>
       </c>
     </row>
-    <row r="38" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A38" s="11">
         <v>37</v>
       </c>
@@ -4445,7 +4445,7 @@
         <v>527</v>
       </c>
     </row>
-    <row r="39" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A39" s="11">
         <v>38</v>
       </c>
@@ -4498,7 +4498,7 @@
         <v>527</v>
       </c>
     </row>
-    <row r="40" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A40" s="11">
         <v>39</v>
       </c>
@@ -4551,7 +4551,7 @@
         <v>527</v>
       </c>
     </row>
-    <row r="41" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A41" s="11">
         <v>40</v>
       </c>
@@ -4604,7 +4604,7 @@
         <v>527</v>
       </c>
     </row>
-    <row r="42" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A42" s="11">
         <v>41</v>
       </c>
@@ -4657,7 +4657,7 @@
         <v>527</v>
       </c>
     </row>
-    <row r="43" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A43" s="11">
         <v>42</v>
       </c>
@@ -4710,7 +4710,7 @@
         <v>527</v>
       </c>
     </row>
-    <row r="44" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A44" s="11">
         <v>43</v>
       </c>
@@ -4763,7 +4763,7 @@
         <v>527</v>
       </c>
     </row>
-    <row r="45" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A45" s="11">
         <v>44</v>
       </c>
@@ -4816,7 +4816,7 @@
         <v>527</v>
       </c>
     </row>
-    <row r="46" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A46" s="11">
         <v>45</v>
       </c>
@@ -4869,7 +4869,7 @@
         <v>527</v>
       </c>
     </row>
-    <row r="47" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A47" s="11">
         <v>46</v>
       </c>
@@ -4922,7 +4922,7 @@
         <v>527</v>
       </c>
     </row>
-    <row r="48" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A48" s="11">
         <v>47</v>
       </c>
@@ -4975,7 +4975,7 @@
         <v>527</v>
       </c>
     </row>
-    <row r="49" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A49" s="11">
         <v>48</v>
       </c>
@@ -5028,7 +5028,7 @@
         <v>527</v>
       </c>
     </row>
-    <row r="50" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A50" s="11">
         <v>49</v>
       </c>
@@ -5081,7 +5081,7 @@
         <v>527</v>
       </c>
     </row>
-    <row r="51" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A51" s="11">
         <v>50</v>
       </c>
@@ -5134,7 +5134,7 @@
         <v>527</v>
       </c>
     </row>
-    <row r="52" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A52" s="11">
         <v>51</v>
       </c>
@@ -5187,7 +5187,7 @@
         <v>527</v>
       </c>
     </row>
-    <row r="53" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A53" s="11">
         <v>52</v>
       </c>
@@ -5240,7 +5240,7 @@
         <v>527</v>
       </c>
     </row>
-    <row r="54" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A54" s="11">
         <v>53</v>
       </c>
@@ -5293,7 +5293,7 @@
         <v>527</v>
       </c>
     </row>
-    <row r="55" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A55" s="11">
         <v>54</v>
       </c>
@@ -5346,7 +5346,7 @@
         <v>527</v>
       </c>
     </row>
-    <row r="56" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A56" s="11">
         <v>55</v>
       </c>
@@ -5399,7 +5399,7 @@
         <v>527</v>
       </c>
     </row>
-    <row r="57" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A57" s="11">
         <v>56</v>
       </c>
@@ -5452,7 +5452,7 @@
         <v>527</v>
       </c>
     </row>
-    <row r="58" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A58" s="11">
         <v>57</v>
       </c>
@@ -5505,7 +5505,7 @@
         <v>527</v>
       </c>
     </row>
-    <row r="59" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A59" s="11">
         <v>58</v>
       </c>
@@ -5558,7 +5558,7 @@
         <v>527</v>
       </c>
     </row>
-    <row r="60" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A60" s="11">
         <v>59</v>
       </c>
@@ -5611,7 +5611,7 @@
         <v>527</v>
       </c>
     </row>
-    <row r="61" spans="1:26" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:26" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A61" s="20">
         <v>60</v>
       </c>
@@ -5673,7 +5673,7 @@
       </c>
       <c r="Z61" s="20"/>
     </row>
-    <row r="62" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A62" s="11">
         <v>61</v>
       </c>
@@ -5726,7 +5726,7 @@
         <v>527</v>
       </c>
     </row>
-    <row r="63" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A63" s="11">
         <v>62</v>
       </c>
@@ -5779,7 +5779,7 @@
         <v>527</v>
       </c>
     </row>
-    <row r="64" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A64" s="11">
         <v>63</v>
       </c>
@@ -5832,7 +5832,7 @@
         <v>527</v>
       </c>
     </row>
-    <row r="65" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A65" s="11">
         <v>64</v>
       </c>
@@ -5885,7 +5885,7 @@
         <v>527</v>
       </c>
     </row>
-    <row r="66" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A66" s="11">
         <v>65</v>
       </c>
@@ -5938,7 +5938,7 @@
         <v>527</v>
       </c>
     </row>
-    <row r="67" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A67" s="11">
         <v>66</v>
       </c>
@@ -5991,7 +5991,7 @@
         <v>527</v>
       </c>
     </row>
-    <row r="68" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A68" s="11">
         <v>67</v>
       </c>
@@ -6044,7 +6044,7 @@
         <v>527</v>
       </c>
     </row>
-    <row r="69" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A69" s="11">
         <v>68</v>
       </c>
@@ -6097,7 +6097,7 @@
         <v>527</v>
       </c>
     </row>
-    <row r="70" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A70" s="11">
         <v>69</v>
       </c>
@@ -6150,7 +6150,7 @@
         <v>527</v>
       </c>
     </row>
-    <row r="71" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A71" s="11">
         <v>70</v>
       </c>
@@ -6203,7 +6203,7 @@
         <v>527</v>
       </c>
     </row>
-    <row r="72" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A72" s="11">
         <v>71</v>
       </c>
@@ -6256,7 +6256,7 @@
         <v>527</v>
       </c>
     </row>
-    <row r="73" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A73" s="11">
         <v>72</v>
       </c>
@@ -6309,7 +6309,7 @@
         <v>527</v>
       </c>
     </row>
-    <row r="74" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A74" s="11">
         <v>73</v>
       </c>
@@ -6362,7 +6362,7 @@
         <v>527</v>
       </c>
     </row>
-    <row r="75" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A75" s="11">
         <v>74</v>
       </c>
@@ -6415,7 +6415,7 @@
         <v>527</v>
       </c>
     </row>
-    <row r="76" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A76" s="11">
         <v>75</v>
       </c>
@@ -6468,7 +6468,7 @@
         <v>527</v>
       </c>
     </row>
-    <row r="77" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A77" s="11">
         <v>76</v>
       </c>
@@ -6521,7 +6521,7 @@
         <v>527</v>
       </c>
     </row>
-    <row r="78" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A78" s="11">
         <v>77</v>
       </c>
@@ -6574,7 +6574,7 @@
         <v>527</v>
       </c>
     </row>
-    <row r="79" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A79" s="11">
         <v>78</v>
       </c>
@@ -6627,7 +6627,7 @@
         <v>527</v>
       </c>
     </row>
-    <row r="80" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A80" s="11">
         <v>79</v>
       </c>
@@ -6680,7 +6680,7 @@
         <v>527</v>
       </c>
     </row>
-    <row r="81" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A81" s="11">
         <v>80</v>
       </c>
@@ -6733,7 +6733,7 @@
         <v>527</v>
       </c>
     </row>
-    <row r="82" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A82" s="11">
         <v>81</v>
       </c>
@@ -6786,7 +6786,7 @@
         <v>527</v>
       </c>
     </row>
-    <row r="83" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A83" s="11">
         <v>82</v>
       </c>
@@ -6839,7 +6839,7 @@
         <v>527</v>
       </c>
     </row>
-    <row r="84" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A84" s="11">
         <v>83</v>
       </c>
@@ -6892,7 +6892,7 @@
         <v>527</v>
       </c>
     </row>
-    <row r="85" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A85" s="11">
         <v>84</v>
       </c>
@@ -6945,7 +6945,7 @@
         <v>527</v>
       </c>
     </row>
-    <row r="86" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A86" s="11">
         <v>85</v>
       </c>
@@ -6998,7 +6998,7 @@
         <v>527</v>
       </c>
     </row>
-    <row r="87" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A87" s="11">
         <v>86</v>
       </c>
@@ -7051,7 +7051,7 @@
         <v>527</v>
       </c>
     </row>
-    <row r="88" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A88" s="11">
         <v>87</v>
       </c>
@@ -7104,7 +7104,7 @@
         <v>527</v>
       </c>
     </row>
-    <row r="89" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A89" s="11">
         <v>88</v>
       </c>
@@ -7157,7 +7157,7 @@
         <v>527</v>
       </c>
     </row>
-    <row r="90" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A90" s="11">
         <v>89</v>
       </c>
@@ -7210,7 +7210,7 @@
         <v>527</v>
       </c>
     </row>
-    <row r="91" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A91" s="11">
         <v>90</v>
       </c>
@@ -7263,7 +7263,7 @@
         <v>527</v>
       </c>
     </row>
-    <row r="92" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A92" s="11">
         <v>91</v>
       </c>
@@ -7316,7 +7316,7 @@
         <v>527</v>
       </c>
     </row>
-    <row r="93" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A93" s="11">
         <v>92</v>
       </c>
@@ -7369,7 +7369,7 @@
         <v>527</v>
       </c>
     </row>
-    <row r="94" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A94" s="11">
         <v>93</v>
       </c>
@@ -7422,7 +7422,7 @@
         <v>527</v>
       </c>
     </row>
-    <row r="95" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A95" s="11">
         <v>94</v>
       </c>
@@ -7475,7 +7475,7 @@
         <v>527</v>
       </c>
     </row>
-    <row r="96" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A96" s="11">
         <v>95</v>
       </c>
@@ -7528,7 +7528,7 @@
         <v>527</v>
       </c>
     </row>
-    <row r="97" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A97" s="11">
         <v>96</v>
       </c>
@@ -7581,7 +7581,7 @@
         <v>527</v>
       </c>
     </row>
-    <row r="98" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A98" s="11">
         <v>97</v>
       </c>
@@ -7634,7 +7634,7 @@
         <v>527</v>
       </c>
     </row>
-    <row r="99" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A99" s="11">
         <v>98</v>
       </c>
@@ -7687,7 +7687,7 @@
         <v>527</v>
       </c>
     </row>
-    <row r="100" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A100" s="11">
         <v>99</v>
       </c>
@@ -7740,7 +7740,7 @@
         <v>527</v>
       </c>
     </row>
-    <row r="101" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A101" s="11">
         <v>100</v>
       </c>
@@ -7793,7 +7793,7 @@
         <v>527</v>
       </c>
     </row>
-    <row r="102" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A102" s="11">
         <v>101</v>
       </c>
@@ -7846,7 +7846,7 @@
         <v>527</v>
       </c>
     </row>
-    <row r="103" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A103" s="11">
         <v>102</v>
       </c>
@@ -7899,7 +7899,7 @@
         <v>527</v>
       </c>
     </row>
-    <row r="104" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A104" s="11">
         <v>103</v>
       </c>
@@ -7952,7 +7952,7 @@
         <v>527</v>
       </c>
     </row>
-    <row r="105" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A105" s="11">
         <v>104</v>
       </c>
@@ -8005,7 +8005,7 @@
         <v>527</v>
       </c>
     </row>
-    <row r="106" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A106" s="11">
         <v>105</v>
       </c>
@@ -8058,7 +8058,7 @@
         <v>527</v>
       </c>
     </row>
-    <row r="107" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A107" s="11">
         <v>106</v>
       </c>
@@ -8111,7 +8111,7 @@
         <v>527</v>
       </c>
     </row>
-    <row r="108" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A108" s="11">
         <v>107</v>
       </c>
@@ -8164,7 +8164,7 @@
         <v>527</v>
       </c>
     </row>
-    <row r="109" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A109" s="11">
         <v>108</v>
       </c>
@@ -8217,7 +8217,7 @@
         <v>527</v>
       </c>
     </row>
-    <row r="110" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A110" s="11">
         <v>109</v>
       </c>
@@ -8270,7 +8270,7 @@
         <v>527</v>
       </c>
     </row>
-    <row r="111" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A111" s="11">
         <v>110</v>
       </c>
@@ -8323,7 +8323,7 @@
         <v>527</v>
       </c>
     </row>
-    <row r="112" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A112" s="11">
         <v>111</v>
       </c>
@@ -8376,7 +8376,7 @@
         <v>527</v>
       </c>
     </row>
-    <row r="113" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A113" s="11">
         <v>112</v>
       </c>
@@ -8429,7 +8429,7 @@
         <v>527</v>
       </c>
     </row>
-    <row r="114" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A114" s="11">
         <v>113</v>
       </c>
@@ -8482,7 +8482,7 @@
         <v>527</v>
       </c>
     </row>
-    <row r="115" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A115" s="11">
         <v>114</v>
       </c>
@@ -8535,7 +8535,7 @@
         <v>527</v>
       </c>
     </row>
-    <row r="116" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A116" s="11">
         <v>115</v>
       </c>
@@ -8588,7 +8588,7 @@
         <v>527</v>
       </c>
     </row>
-    <row r="117" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A117" s="11">
         <v>116</v>
       </c>
@@ -8641,7 +8641,7 @@
         <v>527</v>
       </c>
     </row>
-    <row r="118" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A118" s="11">
         <v>117</v>
       </c>
@@ -8694,7 +8694,7 @@
         <v>527</v>
       </c>
     </row>
-    <row r="119" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A119" s="11">
         <v>118</v>
       </c>
@@ -8747,7 +8747,7 @@
         <v>527</v>
       </c>
     </row>
-    <row r="120" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A120" s="11">
         <v>119</v>
       </c>
@@ -8800,7 +8800,7 @@
         <v>527</v>
       </c>
     </row>
-    <row r="121" spans="1:26" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="121" spans="1:26" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A121" s="20">
         <v>120</v>
       </c>
@@ -8862,7 +8862,7 @@
       </c>
       <c r="Z121" s="20"/>
     </row>
-    <row r="122" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A122" s="11">
         <v>121</v>
       </c>
@@ -8915,7 +8915,7 @@
         <v>527</v>
       </c>
     </row>
-    <row r="123" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A123" s="11">
         <v>122</v>
       </c>
@@ -8968,7 +8968,7 @@
         <v>527</v>
       </c>
     </row>
-    <row r="124" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A124" s="11">
         <v>123</v>
       </c>
@@ -9021,7 +9021,7 @@
         <v>527</v>
       </c>
     </row>
-    <row r="125" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A125" s="11">
         <v>124</v>
       </c>
@@ -9074,7 +9074,7 @@
         <v>527</v>
       </c>
     </row>
-    <row r="126" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A126" s="11">
         <v>125</v>
       </c>
@@ -9127,7 +9127,7 @@
         <v>527</v>
       </c>
     </row>
-    <row r="127" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A127" s="11">
         <v>126</v>
       </c>
@@ -9180,7 +9180,7 @@
         <v>527</v>
       </c>
     </row>
-    <row r="128" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A128" s="11">
         <v>127</v>
       </c>
@@ -9233,7 +9233,7 @@
         <v>527</v>
       </c>
     </row>
-    <row r="129" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A129" s="11">
         <v>128</v>
       </c>
@@ -9286,7 +9286,7 @@
         <v>527</v>
       </c>
     </row>
-    <row r="130" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A130" s="11">
         <v>129</v>
       </c>
@@ -9339,7 +9339,7 @@
         <v>527</v>
       </c>
     </row>
-    <row r="131" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A131" s="11">
         <v>130</v>
       </c>
@@ -9392,7 +9392,7 @@
         <v>527</v>
       </c>
     </row>
-    <row r="132" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A132" s="11">
         <v>131</v>
       </c>
@@ -9445,7 +9445,7 @@
         <v>527</v>
       </c>
     </row>
-    <row r="133" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A133" s="11">
         <v>132</v>
       </c>
@@ -9498,7 +9498,7 @@
         <v>527</v>
       </c>
     </row>
-    <row r="134" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A134" s="11">
         <v>133</v>
       </c>
@@ -9551,7 +9551,7 @@
         <v>527</v>
       </c>
     </row>
-    <row r="135" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="135" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A135" s="11">
         <v>134</v>
       </c>
@@ -9604,7 +9604,7 @@
         <v>527</v>
       </c>
     </row>
-    <row r="136" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="136" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A136" s="11">
         <v>135</v>
       </c>
@@ -9657,7 +9657,7 @@
         <v>527</v>
       </c>
     </row>
-    <row r="137" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="137" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A137" s="11">
         <v>136</v>
       </c>
@@ -9710,7 +9710,7 @@
         <v>527</v>
       </c>
     </row>
-    <row r="138" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="138" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A138" s="11">
         <v>137</v>
       </c>
@@ -9763,7 +9763,7 @@
         <v>527</v>
       </c>
     </row>
-    <row r="139" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="139" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A139" s="11">
         <v>138</v>
       </c>
@@ -9816,7 +9816,7 @@
         <v>527</v>
       </c>
     </row>
-    <row r="140" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="140" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A140" s="11">
         <v>139</v>
       </c>
@@ -9869,7 +9869,7 @@
         <v>527</v>
       </c>
     </row>
-    <row r="141" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="141" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A141" s="11">
         <v>140</v>
       </c>
@@ -9922,7 +9922,7 @@
         <v>527</v>
       </c>
     </row>
-    <row r="142" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="142" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A142" s="11">
         <v>141</v>
       </c>
@@ -9975,7 +9975,7 @@
         <v>527</v>
       </c>
     </row>
-    <row r="143" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="143" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A143" s="11">
         <v>142</v>
       </c>
@@ -10028,7 +10028,7 @@
         <v>527</v>
       </c>
     </row>
-    <row r="144" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="144" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A144" s="11">
         <v>143</v>
       </c>
@@ -10081,7 +10081,7 @@
         <v>527</v>
       </c>
     </row>
-    <row r="145" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="145" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A145" s="11">
         <v>144</v>
       </c>
@@ -10134,7 +10134,7 @@
         <v>527</v>
       </c>
     </row>
-    <row r="146" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="146" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A146" s="11">
         <v>145</v>
       </c>
@@ -10187,7 +10187,7 @@
         <v>527</v>
       </c>
     </row>
-    <row r="147" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="147" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A147" s="11">
         <v>146</v>
       </c>
@@ -10240,7 +10240,7 @@
         <v>527</v>
       </c>
     </row>
-    <row r="148" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="148" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A148" s="11">
         <v>147</v>
       </c>
@@ -10293,7 +10293,7 @@
         <v>527</v>
       </c>
     </row>
-    <row r="149" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="149" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A149" s="11">
         <v>148</v>
       </c>
@@ -10346,7 +10346,7 @@
         <v>527</v>
       </c>
     </row>
-    <row r="150" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="150" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A150" s="11">
         <v>149</v>
       </c>
@@ -10399,7 +10399,7 @@
         <v>527</v>
       </c>
     </row>
-    <row r="151" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="151" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A151" s="11">
         <v>150</v>
       </c>
@@ -10452,7 +10452,7 @@
         <v>527</v>
       </c>
     </row>
-    <row r="152" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="152" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A152" s="11">
         <v>151</v>
       </c>
@@ -10505,7 +10505,7 @@
         <v>527</v>
       </c>
     </row>
-    <row r="153" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="153" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A153" s="11">
         <v>152</v>
       </c>
@@ -10558,7 +10558,7 @@
         <v>527</v>
       </c>
     </row>
-    <row r="154" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="154" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A154" s="11">
         <v>153</v>
       </c>
@@ -10611,7 +10611,7 @@
         <v>527</v>
       </c>
     </row>
-    <row r="155" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="155" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A155" s="11">
         <v>154</v>
       </c>
@@ -10664,7 +10664,7 @@
         <v>527</v>
       </c>
     </row>
-    <row r="156" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="156" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A156" s="11">
         <v>155</v>
       </c>
@@ -10717,7 +10717,7 @@
         <v>527</v>
       </c>
     </row>
-    <row r="157" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="157" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A157" s="11">
         <v>156</v>
       </c>
@@ -10770,7 +10770,7 @@
         <v>527</v>
       </c>
     </row>
-    <row r="158" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="158" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A158" s="11">
         <v>157</v>
       </c>
@@ -10823,7 +10823,7 @@
         <v>527</v>
       </c>
     </row>
-    <row r="159" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="159" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A159" s="11">
         <v>158</v>
       </c>
@@ -10876,7 +10876,7 @@
         <v>527</v>
       </c>
     </row>
-    <row r="160" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="160" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A160" s="11">
         <v>159</v>
       </c>
@@ -10929,7 +10929,7 @@
         <v>527</v>
       </c>
     </row>
-    <row r="161" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="161" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A161" s="11">
         <v>160</v>
       </c>
@@ -10982,7 +10982,7 @@
         <v>527</v>
       </c>
     </row>
-    <row r="162" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="162" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A162" s="11">
         <v>161</v>
       </c>
@@ -11035,7 +11035,7 @@
         <v>527</v>
       </c>
     </row>
-    <row r="163" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="163" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A163" s="11">
         <v>162</v>
       </c>
@@ -11088,7 +11088,7 @@
         <v>527</v>
       </c>
     </row>
-    <row r="164" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="164" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A164" s="11">
         <v>163</v>
       </c>
@@ -11141,7 +11141,7 @@
         <v>527</v>
       </c>
     </row>
-    <row r="165" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="165" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A165" s="11">
         <v>164</v>
       </c>
@@ -11194,7 +11194,7 @@
         <v>527</v>
       </c>
     </row>
-    <row r="166" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="166" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A166" s="11">
         <v>165</v>
       </c>
@@ -11247,7 +11247,7 @@
         <v>527</v>
       </c>
     </row>
-    <row r="167" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="167" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A167" s="11">
         <v>166</v>
       </c>
@@ -11300,7 +11300,7 @@
         <v>527</v>
       </c>
     </row>
-    <row r="168" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="168" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A168" s="11">
         <v>167</v>
       </c>
@@ -11353,7 +11353,7 @@
         <v>527</v>
       </c>
     </row>
-    <row r="169" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="169" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A169" s="11">
         <v>168</v>
       </c>
@@ -11406,7 +11406,7 @@
         <v>527</v>
       </c>
     </row>
-    <row r="170" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="170" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A170" s="11">
         <v>169</v>
       </c>
@@ -11459,7 +11459,7 @@
         <v>527</v>
       </c>
     </row>
-    <row r="171" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="171" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A171" s="11">
         <v>170</v>
       </c>
@@ -11512,7 +11512,7 @@
         <v>527</v>
       </c>
     </row>
-    <row r="172" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="172" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A172" s="11">
         <v>171</v>
       </c>
@@ -11565,7 +11565,7 @@
         <v>527</v>
       </c>
     </row>
-    <row r="173" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="173" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A173" s="11">
         <v>172</v>
       </c>
@@ -11618,7 +11618,7 @@
         <v>527</v>
       </c>
     </row>
-    <row r="174" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="174" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A174" s="11">
         <v>173</v>
       </c>
@@ -11671,7 +11671,7 @@
         <v>527</v>
       </c>
     </row>
-    <row r="175" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="175" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A175" s="11">
         <v>174</v>
       </c>
@@ -11724,7 +11724,7 @@
         <v>527</v>
       </c>
     </row>
-    <row r="176" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="176" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A176" s="11">
         <v>175</v>
       </c>
@@ -11777,7 +11777,7 @@
         <v>527</v>
       </c>
     </row>
-    <row r="177" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="177" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A177" s="11">
         <v>176</v>
       </c>
@@ -11830,7 +11830,7 @@
         <v>527</v>
       </c>
     </row>
-    <row r="178" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="178" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A178" s="11">
         <v>177</v>
       </c>
@@ -11883,7 +11883,7 @@
         <v>527</v>
       </c>
     </row>
-    <row r="179" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="179" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A179" s="11">
         <v>178</v>
       </c>
@@ -11936,7 +11936,7 @@
         <v>527</v>
       </c>
     </row>
-    <row r="180" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="180" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A180" s="11">
         <v>179</v>
       </c>
@@ -11989,7 +11989,7 @@
         <v>527</v>
       </c>
     </row>
-    <row r="181" spans="1:26" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="181" spans="1:26" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A181" s="20">
         <v>180</v>
       </c>
@@ -12070,16 +12070,16 @@
       <selection activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.6640625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="4" width="8.7109375" style="1"/>
-    <col min="5" max="5" width="12.140625" style="1" customWidth="1"/>
-    <col min="6" max="6" width="10.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="10" width="8.7109375" style="1"/>
-    <col min="11" max="16384" width="8.7109375" style="2"/>
+    <col min="1" max="4" width="8.6640625" style="1"/>
+    <col min="5" max="5" width="12.109375" style="1" customWidth="1"/>
+    <col min="6" max="6" width="10.88671875" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="10" width="8.6640625" style="1"/>
+    <col min="11" max="16384" width="8.6640625" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:23" ht="75" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:23" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
@@ -12150,7 +12150,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="2" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:23" x14ac:dyDescent="0.3">
       <c r="H2" s="5"/>
       <c r="I2" s="5"/>
       <c r="J2" s="5"/>
@@ -12168,7 +12168,7 @@
       <c r="V2" s="9"/>
       <c r="W2" s="9"/>
     </row>
-    <row r="3" spans="1:23" ht="45" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:23" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A3" s="1">
         <v>5</v>
       </c>
@@ -12239,7 +12239,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="5" spans="1:23" ht="165" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:23" ht="144" x14ac:dyDescent="0.3">
       <c r="D5" s="1" t="s">
         <v>7</v>
       </c>

</xml_diff>